<commit_message>
running without zero rainfall days
</commit_message>
<xml_diff>
--- a/model-comps/Model_Comps_Split_Nigeria.xlsx
+++ b/model-comps/Model_Comps_Split_Nigeria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amina/Documents/Stanford/precip-price/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amina/Documents/Stanford/precip-price/model-comps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5B744E0F-5926-C241-9143-13FD15B1805A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2EB4CF20-E323-0E47-AB32-769500F1A245}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-7540" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_Comps" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -681,7 +681,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -689,56 +689,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1071,12 +1021,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA44" sqref="AA44"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2:X48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4685,12 +4635,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:R48">
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>D2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:Q48">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>$U2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
saving out final forms
</commit_message>
<xml_diff>
--- a/model-comps/Model_Comps_Split_Nigeria.xlsx
+++ b/model-comps/Model_Comps_Split_Nigeria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amina/Documents/Stanford/precip-price/model-comps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2EB4CF20-E323-0E47-AB32-769500F1A245}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{04118B12-CB04-D142-AC8C-5178A996F789}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1024,9 +1024,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2:X48"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U1" sqref="U1:Z1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>